<commit_message>
Slight changes in table demo columns
</commit_message>
<xml_diff>
--- a/app/tables/plot/forms/plot/plot.xlsx
+++ b/app/tables/plot/forms/plot/plot.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="19660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>data_value</t>
   </si>
   <si>
-    <t>plants</t>
-  </si>
-  <si>
     <t>corn</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Cotton</t>
+  </si>
+  <si>
+    <t>planting</t>
   </si>
 </sst>
 </file>
@@ -256,6 +256,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -583,18 +588,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -617,7 +622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -632,7 +637,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -647,7 +652,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -662,7 +667,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>25</v>
@@ -671,7 +676,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -696,12 +701,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -712,37 +717,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -760,18 +765,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -782,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -790,7 +795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -798,7 +803,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -806,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Change to make plot and visit forms more consistent
</commit_message>
<xml_diff>
--- a/app/tables/plot/forms/plot/plot.xlsx
+++ b/app/tables/plot/forms/plot/plot.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500"/>
+    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>type</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>planting</t>
+  </si>
+  <si>
+    <t>plot_name</t>
   </si>
 </sst>
 </file>
@@ -588,18 +591,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -622,7 +625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -637,14 +640,14 @@
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -652,7 +655,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -667,7 +670,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>25</v>
@@ -701,12 +704,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -717,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -728,7 +731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -739,7 +742,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -765,18 +768,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -787,7 +790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -795,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -803,7 +806,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -811,12 +814,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge. haven't tested with new forms.
</commit_message>
<xml_diff>
--- a/app/tables/plot/forms/plot/plot.xlsx
+++ b/app/tables/plot/forms/plot/plot.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500"/>
+    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>type</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>planting</t>
+  </si>
+  <si>
+    <t>plot_name</t>
   </si>
 </sst>
 </file>
@@ -588,18 +591,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -622,7 +625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -637,14 +640,14 @@
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -652,7 +655,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -667,7 +670,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>25</v>
@@ -701,12 +704,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -717,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -728,7 +731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -739,7 +742,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -765,18 +768,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -787,7 +790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -795,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -803,7 +806,7 @@
         <v>20140331</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -811,12 +814,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up plot.xlsx for demo
</commit_message>
<xml_diff>
--- a/app/tables/plot/forms/plot/plot.xlsx
+++ b/app/tables/plot/forms/plot/plot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="6560" windowWidth="25600" windowHeight="16220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>type</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>display.text</t>
-  </si>
-  <si>
-    <t>display.hint</t>
-  </si>
-  <si>
-    <t>hideInContents</t>
   </si>
   <si>
     <t>text</t>
@@ -589,22 +583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -618,71 +611,59 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="6"/>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -711,10 +692,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -722,35 +703,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +750,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -781,26 +762,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>20140331</v>
@@ -808,18 +789,18 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the files for the previous gates demo.
</commit_message>
<xml_diff>
--- a/app/tables/plot/forms/plot/plot.xlsx
+++ b/app/tables/plot/forms/plot/plot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -38,9 +38,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -80,12 +77,6 @@
     <t>Plot</t>
   </si>
   <si>
-    <t>plot_id</t>
-  </si>
-  <si>
-    <t>Enter the id of plot:</t>
-  </si>
-  <si>
     <t>instance_name</t>
   </si>
   <si>
@@ -126,6 +117,9 @@
   </si>
   <si>
     <t>plot_name</t>
+  </si>
+  <si>
+    <t>table_id</t>
   </si>
 </sst>
 </file>
@@ -583,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,7 +591,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -615,55 +609,42 @@
     <row r="2" spans="1:5">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6"/>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6"/>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -692,10 +673,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -703,35 +684,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -747,10 +728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -762,26 +743,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>20140331</v>
@@ -789,18 +770,26 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>